<commit_message>
giao diện giỏ hàng
</commit_message>
<xml_diff>
--- a/SQL/Book1.xlsx
+++ b/SQL/Book1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chien\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DH_CNDA\DACN1\DACN1\SQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3ECA92-E829-45CF-97B8-EEEFE2C7976E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70E38B6-4FAA-4497-9219-1D752C9782B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5448" yWindow="2316" windowWidth="9312" windowHeight="12192" xr2:uid="{4768B4C4-959E-4FA0-B170-91749BDB7074}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{4768B4C4-959E-4FA0-B170-91749BDB7074}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="115">
   <si>
     <t>admin</t>
   </si>
@@ -765,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8585E7D5-6979-47FB-AB11-8183615A8D56}">
   <dimension ref="A1:K97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1843,7 +1843,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>57</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>58</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>59</v>
       </c>
@@ -1867,7 +1867,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>60</v>
       </c>
@@ -1875,65 +1875,83 @@
         <v>61</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="86" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>73</v>
       </c>
       <c r="B86" s="5" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C86" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>81</v>
       </c>
       <c r="B87">
         <v>2</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>81</v>
       </c>
       <c r="B88">
         <v>3</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C88">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>57</v>
       </c>
       <c r="B89">
         <v>5</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>57</v>
       </c>
       <c r="B90">
         <v>4</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C90">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>58</v>
       </c>
       <c r="B91">
         <v>3</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="93" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>1</v>
       </c>
@@ -1941,7 +1959,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>1</v>
       </c>
@@ -1949,7 +1967,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>2</v>
       </c>
@@ -1957,7 +1975,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
chức năng thanh toans post man
</commit_message>
<xml_diff>
--- a/SQL/Book1.xlsx
+++ b/SQL/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DH_CNDA\DACN1\DACN1\SQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E1322F-7A99-461D-821C-182D9E2883FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E778C3-D7DC-4ECD-BDB9-9DDFB97C1429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4768B4C4-959E-4FA0-B170-91749BDB7074}"/>
   </bookViews>
@@ -762,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8585E7D5-6979-47FB-AB11-8183615A8D56}">
   <dimension ref="A1:K98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O43" sqref="O43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>